<commit_message>
update titlte payment status
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/DebitAmountDetailByContract.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/DebitAmountDetailByContract.xlsx
@@ -102,9 +102,6 @@
     <t>Service</t>
   </si>
   <si>
-    <t>Invoice Payment Status</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>{SumTotalUSD}</t>
+  </si>
+  <si>
+    <t>Payment Status</t>
   </si>
 </sst>
 </file>
@@ -392,15 +392,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -413,6 +404,15 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,8 +744,8 @@
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="23" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="26" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
@@ -757,7 +757,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="19" t="s">
         <v>0</v>
       </c>
     </row>
@@ -766,13 +766,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -780,13 +780,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -794,13 +794,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -825,10 +825,10 @@
       <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="27" t="s">
         <v>15</v>
       </c>
       <c r="J7" s="17" t="s">
@@ -850,75 +850,75 @@
         <v>21</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="I8" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="J8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="Q8" s="8"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="26" t="s">
+      <c r="A9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>53</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
@@ -930,24 +930,24 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="30" t="s">
         <v>50</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -960,18 +960,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,18 +1178,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F4E6D7-2173-4855-B72E-B454B205DDA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F66DAAF6-2D09-4A7A-98BC-D382A08213D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F66DAAF6-2D09-4A7A-98BC-D382A08213D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F4E6D7-2173-4855-B72E-B454B205DDA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>